<commit_message>
update mapping scheme of industrial buildings Turkey to include CR/LFM
</commit_message>
<xml_diff>
--- a/ind_mapping_schemes/mapping_Turkey_IND.xlsx
+++ b/ind_mapping_schemes/mapping_Turkey_IND.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/Exposure_model_validation/ind_mapping_schemes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/ind_mapping_schemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CC1437-7FE6-3646-92F0-83D7F593956E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A64217-0968-8840-98B8-F97ED7080A0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="880" windowWidth="25240" windowHeight="13220" xr2:uid="{C8C05C96-D893-E341-8FBD-8F9D4DE94777}"/>
+    <workbookView xWindow="2300" yWindow="1220" windowWidth="25240" windowHeight="13220" xr2:uid="{C8C05C96-D893-E341-8FBD-8F9D4DE94777}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_istanbul" sheetId="2" r:id="rId1"/>
@@ -99,17 +99,6 @@
     <t>100% S/LFM+CDL/HBET:1-3</t>
   </si>
   <si>
-    <t>60% CR/LFINF+CDL/HBET:1-3
-40% CR/LFINF+CDL/HBET:4-6</t>
-  </si>
-  <si>
-    <t>100% CR/LFINF(CBH)+CDL/HBET:1-3</t>
-  </si>
-  <si>
-    <t>70% CR/LFINF(CL)+CDL/HBET:1-3
-30% CR/LFINF(CL)+CDL/HBET:4-6</t>
-  </si>
-  <si>
     <t>100% W/LFM+CDL/HBET:1-3</t>
   </si>
   <si>
@@ -128,14 +117,7 @@
     <t>100% CR/LDUAL+CDL/HBET:1-3</t>
   </si>
   <si>
-    <t>100% CR+PC/LWAL+CDL/HBET:1-3</t>
-  </si>
-  <si>
     <t>100% SRC/LFM+CDH/HBET:1-3</t>
-  </si>
-  <si>
-    <t>80% CR/LFINF(CL)+CDL/HBET:1-3
-20% CR/LFINF(CL)+CDL/HBET:4-6</t>
   </si>
   <si>
     <t>80% CR/LWAL+CDL/HBET:1-3
@@ -146,12 +128,30 @@
 20% CR/LDUAL+CDL/HBET:4-6</t>
   </si>
   <si>
-    <t>80% CR+PC/LWAL+CDL/HBET:1-3
-20% CR+PC/LWAL+CDL/HBET:4-6</t>
-  </si>
-  <si>
     <t>80% SRC/LFM+CDH/HBET:1-3
 20% SRC/LFM+CDH/HBET:4-6</t>
+  </si>
+  <si>
+    <t>80% CR+PC/LFM+CDL/HBET:1-3
+20% CR+PC/LFM+CDL/HBET:4-6</t>
+  </si>
+  <si>
+    <t>100% CR+PC/LFM+CDL/HBET:1-3</t>
+  </si>
+  <si>
+    <t>60% CR/LFM+CDL/HBET:1-3
+40% CR/LFM+CDL/HBET:4-6</t>
+  </si>
+  <si>
+    <t>80% CR/LFM+CDL/HBET:1-3
+20% CR/LFM+CDL/HBET:4-6</t>
+  </si>
+  <si>
+    <t>100% CR/LFM+CDL/HBET:1-3</t>
+  </si>
+  <si>
+    <t>70% CR/LFM+CDL/HBET:1-3
+30% CR/LFM+CDL/HBET:4-6</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:CV2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -679,49 +679,49 @@
         <v>17</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="H2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="O2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -816,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED03CA62-BFCC-0B43-90D1-CC2B32AC668A}">
   <dimension ref="A1:CV2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -901,49 +901,49 @@
         <v>17</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="I2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="M2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>

</xml_diff>